<commit_message>
excel file and pdf sample added
</commit_message>
<xml_diff>
--- a/meta_data/ptsplant.xlsx
+++ b/meta_data/ptsplant.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t xml:space="preserve">Plant name</t>
   </si>
@@ -50,58 +50,61 @@
     <t xml:space="preserve">home plant</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/seenuvasan1947/ptsplant-data/raw/main/meta_data/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mango</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyzmango</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lumped,tb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diseases name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plant may affect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wheather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fileurl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">january</t>
+  </si>
+  <si>
+    <t xml:space="preserve">over cold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paracetamol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rainy</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://github.com/seenuvasan1947/ptsplant-data/raw/main/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mango</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xyzmango</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lumped,tb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diseases name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cause</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medicine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plant may affect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wheather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fileurl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">january</t>
-  </si>
-  <si>
-    <t xml:space="preserve">over cold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paracetamol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rainy</t>
   </si>
   <si>
     <t xml:space="preserve">cancer</t>
@@ -159,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -193,12 +196,6 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -244,7 +241,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,6 +254,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,14 +267,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -297,10 +290,10 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.5"/>
@@ -320,7 +313,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -337,7 +330,7 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -348,20 +341,20 @@
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://github.com/seenuvasan1947/ptsplant-data/raw/main/"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://github.com/seenuvasan1947/ptsplant-data/raw/main/"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://github.com/seenuvasan1947/ptsplant-data/raw/main/meta_data/"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://github.com/seenuvasan1947/ptsplant-data/raw/main/meta_data/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -384,126 +377,126 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>9</v>
+      <c r="G2" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>9</v>
+      <c r="F4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>9</v>
+      <c r="F5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>9</v>
+      <c r="F6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>